<commit_message>
Afegeix efecte de focs artificials quan es revela la casa del membre
Implementa un efecte visual de focs artificials que es dispara quan es mostra la categoria/casa assignada a cada membre. L'efecte utilitza el color específic de cada casa i crea múltiples explosions amb partícules que s'expandeixen i s'esvaeixen gradualment.
</commit_message>
<xml_diff>
--- a/barret_magic_muixeranga_COMPLET.xlsx
+++ b/barret_magic_muixeranga_COMPLET.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,7 +427,7 @@
         <v>Gabri</v>
       </c>
       <c r="C2" t="str">
-        <v>Gabriel… tanta pau, seny i patxamama només poden anar a una casa: el barret et fa…</v>
+        <v>Gabriel… el nostre Presi. Tanta pau, seny i patxamama només poden anar a una casa: el barret et fa tancar els ulls un moment abans de revelar el seu destí…</v>
       </c>
       <c r="D2" t="str">
         <v>President de la colla, representa la patxamama i el saber-estar, el seny, mai la rauxa.</v>
@@ -444,7 +444,7 @@
         <v>Míriam</v>
       </c>
       <c r="C3" t="str">
-        <v>Míriam… cos petit, cor enorme i sempre amunt: el barret et veu com una…</v>
+        <v>Míriam… cos petit, cor enorme i sempre amunt: el barret et veu com una companya imprescindible quan tot s’enfila cap al cel…</v>
       </c>
       <c r="D3" t="str">
         <v>Petita alçadora amb un cor molt gran, forma part de la Junta i és la vicepresidenta.</v>
@@ -461,7 +461,7 @@
         <v>Laia</v>
       </c>
       <c r="C4" t="str">
-        <v>Laia Classic… somriure etern i alçades impecables: el barret et col·loca a…</v>
+        <v>Laia Classic… somriure etern i alçades impecables: el barret et col·loca a un racó on l’energia mai cau i els nervis es tornen riures…</v>
       </c>
       <c r="D4" t="str">
         <v>D’Algemesí, alçadora d’una categoria espectacular, bona gent i sempre amb un somriure.</v>
@@ -478,7 +478,7 @@
         <v>Marta</v>
       </c>
       <c r="C5" t="str">
-        <v>Marta Peris… mestra de persones i figures, sempre al peu del canó: el barret t’assenyala clarament com a…</v>
+        <v>Marta Peris… mestra de persones i figures, sempre al peu del canó: el barret t’assenyala clarament com a ànima tranquil·la enmig de la tempesta…</v>
       </c>
       <c r="D5" t="str">
         <v>Mestra de la colla, sempre amb un somriure, una paraula amable i cuidant a la gent.</v>
@@ -495,7 +495,7 @@
         <v>Iván</v>
       </c>
       <c r="C6" t="str">
-        <v>Iván Garnelo… idees infinites i paraules sense límit: el barret et deixa a…</v>
+        <v>Iván Garnelo… idees infinites i paraules sense límit: el barret et deixa al centre del soroll, on les xapes es convertixen en saviesa compartida…</v>
       </c>
       <c r="D6" t="str">
         <v>Últim guanyador del Premi Xapes, molt disposat a treballar per la colla, molt intel·ligent i molt bona persona, però un poquet xapes, sempre parlant.</v>
@@ -512,7 +512,7 @@
         <v>Moliner</v>
       </c>
       <c r="C7" t="str">
-        <v>Eva Moliner… qui cuida la xicalla cuida el futur: el barret t’abraça i et declara…</v>
+        <v>Eva Moliner… qui cuida la xicalla cuida el futur: el barret t’abraça i et recorda que sense tu moltes figures ni tan sols començarien…</v>
       </c>
       <c r="D7" t="str">
         <v>Cap de xicalla, cuida els xiquets i xiquetes i millora constantment per fer les millors figures.</v>
@@ -529,7 +529,7 @@
         <v>Pepelu</v>
       </c>
       <c r="C8" t="str">
-        <v>Pepelu… carisma, família i valors muixeranguers forts: el barret no dubta, ets…</v>
+        <v>Pepelu… carisma, família i valors muixeranguers forts: el barret no dubta, veu en tu aquell que aguanta el projecte quan tot tremola…</v>
       </c>
       <c r="D8" t="str">
         <v>Pare de Pol i Joan, home carismàtic, entregat i amb uns valors muixeranguers molt grans.</v>
@@ -546,7 +546,7 @@
         <v>Carles</v>
       </c>
       <c r="C9" t="str">
-        <v>Carles… cada núvol, cada festa i cada figura passen pel teu radar: el barret et proclama…</v>
+        <v>Carles… cada núvol, cada festa i cada figura passen pel teu radar: el barret et proclama narrador oficial de la colla, meteoròleg de la nit i del bon humor…</v>
       </c>
       <c r="D9" t="str">
         <v>Personatge de la colla, el més divertit i xerraina, meteoròleg de capçalera, sempre amb alguna cosa per explicar.</v>
@@ -563,7 +563,7 @@
         <v>Roger</v>
       </c>
       <c r="C10" t="str">
-        <v>Roger… nou però ja imprescindible, compromès i rialler: el barret et veu com un…</v>
+        <v>Roger… nou però ja imprescindible, compromès i rialler: el barret et veu com un somriure recent arribat que ja sembla de tota la vida…</v>
       </c>
       <c r="D10" t="str">
         <v>Talent emergent molt compromès, català i molt divertit, sempre amb un somriure a la cara.</v>
@@ -580,7 +580,7 @@
         <v>Joanot</v>
       </c>
       <c r="C11" t="str">
-        <v>Joanot… alçada, memes i amor per la terra: el barret et llança directe a…</v>
+        <v>Joanot… alçada, memes i amor per la terra: el barret et llança directe al centre del convit, on mai falta festa ni pinya ni crits de la Safor i Castelló…</v>
       </c>
       <c r="D11" t="str">
         <v>Castellonenc, enamorat del País Valencià i de Catalunya, cap de pinyes, dels més alts de la colla, una ‘loca’ estimada, rei dels memes i molt divertit; referent des de fa anys.</v>
@@ -597,7 +597,7 @@
         <v>Jordi</v>
       </c>
       <c r="C12" t="str">
-        <v>“Jordi… memes infinits, pinyes i festa fins al final: el barret et proclama…”</v>
+        <v>“Jordi… memes infinits, pinyes i festa fins al final: el barret et proclama veu de fons de totes les nits llargues de la colla…”</v>
       </c>
       <c r="D12" t="str">
         <v>Rei dels memes, tothom vol escoltar-lo perquè sempre hi ha alguna cosa graciosa darrere de les seues paraules; cap de pinyes i enamorat del projecte des de fa temps; molt estimat i sempre fins al final de les festes.</v>
@@ -614,7 +614,7 @@
         <v>Celia</v>
       </c>
       <c r="C13" t="str">
-        <v>Celia… somriure, creixement i lluita feminista: el barret et veu com un…</v>
+        <v>Celia… somriure, creixement i lluita feminista: el barret et veu com un far petit però constant que il·lumina camins nous…</v>
       </c>
       <c r="D13" t="str">
         <v>Talent emergent, evoluciona molt ràpidament, sempre amb un somriure i forma part de la comissió feminista.</v>
@@ -631,7 +631,7 @@
         <v>Meritxell</v>
       </c>
       <c r="C14" t="str">
-        <v>Meritxell… cap i cor al servei de la llengua i de la colla: el barret et deixa a la casa…</v>
+        <v>Meritxell… cap i cor al servei de la llengua i de la colla: el barret et deixa a la casa on es guarden les paraules que mai no volem perdre…</v>
       </c>
       <c r="D14" t="str">
         <v>Psicòloga, enamorada del País Valencià i defensora de la llengua; des del principi ha aportat moltíssim a la colla.</v>
@@ -648,7 +648,7 @@
         <v>Montserrat</v>
       </c>
       <c r="C15" t="str">
-        <v>Albert Montserrat… pont entre muixiganga i muixeranga: el barret et tria…</v>
+        <v>Albert Montserrat… pont entre muixiganga i muixeranga: el barret et tria com a viatger de tradicions que no es cansen mai de reinventar-se…</v>
       </c>
       <c r="D15" t="str">
         <v>Home curiós de Sitges que comparteix la seua muixiganga, una cultura de tors humans molt arrelada i diferent però germana.</v>
@@ -665,7 +665,7 @@
         <v>Tere</v>
       </c>
       <c r="C16" t="str">
-        <v>Tere Pitarch… origen, arrels i projecte de vida: el barret et corona com a…</v>
+        <v>Tere Pitarch… origen, arrels i projecte de vida: el barret et corona com a memòria viva d’allò que mai hauríem d’oblidar…</v>
       </c>
       <c r="D16" t="str">
         <v>Tere, mestra fa quatre anys, amb valors muixeranguers molt arrelats; persona seriosa però divertida, gaudeix molt del projecte que va ajudar a crear fa set anys.</v>
@@ -682,7 +682,7 @@
         <v>Miquel</v>
       </c>
       <c r="C17" t="str">
-        <v>Miquel… nervis, xapes i amor infinit per la colla: el barret t’abraça fort i et deixa a…</v>
+        <v>Miquel… nervis, xapes i amor infinit per la colla: el barret t’abraça fort i et deixa al lloc on les idees boges es converteixen en realitat any rere any…</v>
       </c>
       <c r="D17" t="str">
         <v>Primer mestre de la muixeranga i ànima d’aquesta dinàmica; nerviós i una mica xapes, però qui més estima el projecte.</v>
@@ -699,7 +699,7 @@
         <v>Peña</v>
       </c>
       <c r="C18" t="str">
-        <v>Peña… explosió d’energia, pinya i il·lusió tècnica: el barret et veu com un…</v>
+        <v>Peña… explosió d’energia, pinya i il·lusió tècnica: el barret et veu com un motor encés que no sap què és el fre…</v>
       </c>
       <c r="D18" t="str">
         <v>Cap de pinyes, caràcter explosiu, enamorada de la muixeranga, molt optimista i gran talent emergent ja dins l’equip tècnic.</v>
@@ -716,7 +716,7 @@
         <v>Bolu</v>
       </c>
       <c r="C19" t="str">
-        <v>Irene Bolu… reptes, energia i futur als ulls: el barret et tria com a…</v>
+        <v>Irene Bolu… reptes, energia i futur als ulls: el barret et tria com a promesa que ja comença a sonar a confirmació…</v>
       </c>
       <c r="D19" t="str">
         <v>Talent emergent coneguda l’any passat i que enguany es desenvolupa molt ràpidament, aconseguint reptes; és la joventut i energia que necessita la colla.</v>
@@ -733,7 +733,7 @@
         <v>Borrell</v>
       </c>
       <c r="C20" t="str">
-        <v>David Borrell… alçada, barri i lluita: el barret et fa…</v>
+        <v>David Borrell… alçada, barri i lluita: el barret et fa recordar que hi ha columnes que sostenen molt més que una simple figura…</v>
       </c>
       <c r="D20" t="str">
         <v>Un dels més alts de la colla, molt bona persona, de la Barceloneta, molt català i sempre en lluita.</v>
@@ -750,7 +750,7 @@
         <v>Alberto</v>
       </c>
       <c r="C21" t="str">
-        <v>Alberto… nou, fort i amb ganes de festa: el barret et veu claríssim com a…</v>
+        <v>Alberto… nou, fort i amb ganes de festa: el barret et veu claríssim com a fitxatge d’hivern que ha vingut per quedar-se…</v>
       </c>
       <c r="D21" t="str">
         <v>Talent emergent arribat enguany amb molta força; primeres mans segures i gran afició a la festa.</v>
@@ -767,7 +767,7 @@
         <v>De Luis</v>
       </c>
       <c r="C22" t="str">
-        <v>Laura de Luis… petita tempesta de riures, idees i ajuda: el barret et posa a…</v>
+        <v>Laura de Luis… petita tempesta de riures, idees i ajuda: el barret et posa a la zona on es cuinen els plans més bojos i necessaris…</v>
       </c>
       <c r="D22" t="str">
         <v>Companya de la dinàmica, petita i divertida, sempre ajudant la colla i capaç d’arrencar un somriure a tothom; forma part de la Junta i de la Comissió Tecnològica.</v>
@@ -784,7 +784,7 @@
         <v>Adri</v>
       </c>
       <c r="C23" t="str">
-        <v>Adri… bits, bromes i alçades de Tenerife: el barret et col·loca a…</v>
+        <v>Adri… bits, bromes i alçades de Tenerife: el barret et col·loca allà on el wifi, la rialla i la faixa es troben a mig camí…</v>
       </c>
       <c r="D23" t="str">
         <v>Canari de Tenerife, tecnològic i molt divertit; el número 23 és la seua alçada.</v>
@@ -801,7 +801,7 @@
         <v>Mònica</v>
       </c>
       <c r="C24" t="str">
-        <v>Mònica… cada figura al teu cap i cada persona al teu cor: el barret t’assenyala com a…</v>
+        <v>Mònica… cada figura al teu cap i cada persona al teu cor: el barret t’assenyala com a arquitecta silenciosa del que passa a plaça…</v>
       </c>
       <c r="D24" t="str">
         <v>Mestra molt compromesa amb tota la colla, es trenca el cap perquè tothom participe i perquè la muixeranga arribe tan alt com ampla a la plaça.</v>
@@ -818,7 +818,7 @@
         <v>Fadi</v>
       </c>
       <c r="C25" t="str">
-        <v>Fadi… d’Armènia a la plaça, entre memes i reptes nous: el barret et veu com a…</v>
+        <v>Fadi… d’Armènia a la plaça, entre memes i reptes nous: el barret et veu com a viatger intrèpid que ja ha trobat una segona casa…</v>
       </c>
       <c r="D25" t="str">
         <v>D’Armènia, casteller que s’ha sumat a la muixeranga i ja forma part del camí on vol arribar la colla; sempre porta algun meme.</v>
@@ -835,7 +835,7 @@
         <v>Ester</v>
       </c>
       <c r="C26" t="str">
-        <v>Ester… botes posades, festa a punt i ganes d’encadenar partits i figures: el barret et veu com a…</v>
+        <v>Ester… botes posades, festa a punt i ganes d’encadenar partits i figures: el barret et veu com a esportista de llarg recorregut també entre faixes…</v>
       </c>
       <c r="D26" t="str">
         <v>Futbolista i talent emergent que ve acompanyada i sempre molt festera.</v>
@@ -852,7 +852,7 @@
         <v>Luca</v>
       </c>
       <c r="C27" t="str">
-        <v>Luca… pasta, troncs i cos entregat a la colla: el barret et proclama…</v>
+        <v>Luca… pasta, troncs i cos entregat a la colla: el barret et proclama cuiner d’històries i pilars, sempre al centre del foc…</v>
       </c>
       <c r="D27" t="str">
         <v>L’italià de la colla, sempre té alguna cosa per cuinar i és cap de troncs; té molts valors muixeranguers i diu que ha entregat el seu cos a la muixeranga.</v>
@@ -869,7 +869,7 @@
         <v>Lluïsa</v>
       </c>
       <c r="C28" t="str">
-        <v>Lluïsa… abraçades, troncs i compromís fins al cim: el barret et fa…</v>
+        <v>Lluïsa… abraçades, troncs i compromís fins al cim: el barret et fa tancar files al teu voltant, perquè tothom sap que al teu costat s’hi està segur…</v>
       </c>
       <c r="D28" t="str">
         <v>Cap de troncs de la Vilatge Oyosa, Marina Baixa; xiqueta que tothom voldria abraçar, molt agradable, amable i compromesa amb el projecte.</v>
@@ -886,7 +886,7 @@
         <v>Rafel</v>
       </c>
       <c r="C29" t="str">
-        <v>Rafel… agendes, contactes i cultura de barri: el barret et posa a…</v>
+        <v>Rafel… agendes, contactes i cultura de barri: el barret et posa a la xarxa invisible que fa possible festes, actuacions i trobades improbables…</v>
       </c>
       <c r="D29" t="str">
         <v>L’home amb més contactes del barri de Sants, ha donat un valor importantíssim a la colla i fa veure l’activitat des d’un prisma molt cultural.</v>
@@ -903,7 +903,7 @@
         <v>Laiuski</v>
       </c>
       <c r="C30" t="str">
-        <v>Laiuski… xicalla, compromís i futur als ulls: el barret et tria com a…</v>
+        <v>Laiuski… xicalla, compromís i futur als ulls: el barret et tria com a exemple que el demà ja ha arribat i porta faixa…</v>
       </c>
       <c r="D30" t="str">
         <v>De la Font del Carròs, nou talent emergent de l’any passat, molt compromesa amb la xicalla i amb moltes ganes de seguir; la Iusqui és futur de la colla.</v>
@@ -920,7 +920,7 @@
         <v>Clara</v>
       </c>
       <c r="C31" t="str">
-        <v>Clara… cada xiquet al cor i un somriure per a cadascú: el barret et veu…</v>
+        <v>Clara… cada xiquet al cor i un somriure per a cadascú: el barret et veu custodiant la porta d’entrada de la colla més petita…</v>
       </c>
       <c r="D31" t="str">
         <v>Cap de xicalla, un amor empàtic, molt compromesa amb tots els xiquets i sempre amb un somriure.</v>
@@ -937,7 +937,7 @@
         <v>Olga</v>
       </c>
       <c r="C32" t="str">
-        <v>Olga… de València a Barcelona, dolçor i xicalla a parts iguals: el barret et tria…</v>
+        <v>Olga… de València a Barcelona, dolçor i xicalla a parts iguals: el barret et tria com a pont de sucre entre dos territoris germans…</v>
       </c>
       <c r="D32" t="str">
         <v>Muixeranguera de la Muixeranga de València enamorada de la Muixeranga de Barcelona; cap de xicalla i molt dolceta.</v>
@@ -954,7 +954,7 @@
         <v>Sofia</v>
       </c>
       <c r="C33" t="str">
-        <v>Sofia… troncs ferms i amabilitat infinita: el barret et posa a…</v>
+        <v>Sofia… troncs ferms i amabilitat infinita: el barret et posa en aquella línia fina on la força i la tendresa es donen la mà…</v>
       </c>
       <c r="D33" t="str">
         <v>Forma part de l’equip de troncs; tan amable que impressiona, sempre té una paraula amable i està disposada a ajudar; l’any passat va ser talent emergent de la colla.</v>
@@ -971,7 +971,7 @@
         <v>Neusin</v>
       </c>
       <c r="C34" t="str">
-        <v>Neusin… terratrèmol d’amor, emoció i xicalla: el barret et veu…</v>
+        <v>Neusin… terratrèmol d’amor, emoció i xicalla: el barret et veu com una abraçada que arriba abans fins i tot que les paraules…</v>
       </c>
       <c r="D34" t="str">
         <v>Terremoto amorós, cap de xicalla i molt emocional; la muixeranga és un projecte que s’ha fet seu i que l’ha fet créixer molt; sempre disposada a ajudar.</v>
@@ -988,7 +988,7 @@
         <v>Pere</v>
       </c>
       <c r="C35" t="str">
-        <v>Pere… tabal, cuina i bon ambient allà on vas: el barret et declara…</v>
+        <v>Pere… tabal, cuina i bon ambient allà on vas: el barret et declara responsable oficial de que mai falte ni ritme ni forqueta…</v>
       </c>
       <c r="D35" t="str">
         <v>Tabal de la colla de tabals i xirimites, sempre ajuda a cuinar i a passar-ho bé; és un home molt de la colla.</v>
@@ -1005,7 +1005,7 @@
         <v>Josep</v>
       </c>
       <c r="C36" t="str">
-        <v>Josep Grau… fundador, valors i respecte en cada pas: el barret et proclama…</v>
+        <v>Josep Grau… fundador, valors i respecte en cada pas: el barret et proclama brúixola discreta que sempre marca el nord de la colla…</v>
       </c>
       <c r="D36" t="str">
         <v>Fundador de la colla, representa els valors muixeranguers per davant de tot; molt amable, respecta sempre qui està al capdavant i quan opina ho fa amb molta cura.</v>
@@ -1022,7 +1022,7 @@
         <v>José</v>
       </c>
       <c r="C37" t="str">
-        <v>José la Rubia… acollida andalusa i alegria granadina: el barret et col·loca a…</v>
+        <v>José la Rubia… acollida andalusa i alegria granadina: el barret et col·loca a la porta d’entrada on ningú se sent estrany ni el primer dia…</v>
       </c>
       <c r="D37" t="str">
         <v>Andalús granadí molt divertit, sempre té una frase amable i una acollida per a tothom; forma part de la comissió d’acollida i rep les noves persones amb molta alegria.</v>
@@ -1039,7 +1039,7 @@
         <v>Guille</v>
       </c>
       <c r="C38" t="str">
-        <v>Guille... vas i véns de la tècnica, però mai de la colla: el barret et fa…</v>
+        <v>Guille... vas i véns de la tècnica, però mai de la colla: el barret et fa guardian silenciós que apareix just quan fa falta una mà més…</v>
       </c>
       <c r="D38" t="str">
         <v>S’ha deixat la tècnica dues vegades, però sempre està ahí esperant que li demanen qualsevol cosa per ajudar; suport constant des de fora de focus.</v>
@@ -1056,7 +1056,7 @@
         <v>Victòria</v>
       </c>
       <c r="C39" t="str">
-        <v>Victòria… compromís, família i mirada feminista: el barret et tria…</v>
+        <v>Victòria… compromís, família i mirada feminista: el barret et tria com a veu serena que recorda per què fem el que fem…</v>
       </c>
       <c r="D39" t="str">
         <v>Molt compromesa des de l’any passat, forma part de la comissió feminista i ve en família a la muixeranga, sempre amb un to molt amable.</v>
@@ -1073,7 +1073,7 @@
         <v>Sandra</v>
       </c>
       <c r="C40" t="str">
-        <v>Sandra… elevadora revelació i figures que fan història: el barret et veu com a…</v>
+        <v>Sandra… elevadora revelació i figures que fan història: el barret et veu com a peça clau d’aquelles fotos que mirarem d’aquí uns anys…</v>
       </c>
       <c r="D40" t="str">
         <v>Talent emergent que va començar l’any passat; elevadora revelació que ha posat en el mapa el jinete Terra de muixerangues.</v>
@@ -1090,7 +1090,7 @@
         <v>Juds</v>
       </c>
       <c r="C41" t="str">
-        <v>Juds… bata invisible, cures i riure contagiós: el barret et declara…</v>
+        <v>Juds… bata invisible, cures i riure contagiós: el barret et declara escut sanitari i emocional a parts iguals…</v>
       </c>
       <c r="D41" t="str">
         <v>Forma part de la comissió sanitària, catalana de l’Hospitalet, amb un riure molt contagiós; cuida de tota la colla a nivell de salut.</v>
@@ -1107,7 +1107,7 @@
         <v>Maria</v>
       </c>
       <c r="C42" t="str">
-        <v>Maria Díez… alçada basca i empenta feminista: el barret et col·loca a…</v>
+        <v>Maria Díez… alçada basca i empenta feminista: el barret et col·loca a la línia on el cos obre camí per a moltes altres dones…</v>
       </c>
       <c r="D42" t="str">
         <v>La nòvia més alta de la colla, d’Euskal Herria; ha posat en valor la muixeranga al País Basc i ha ajudat a fer figures de dones que abans no es feien.</v>
@@ -1124,7 +1124,7 @@
         <v>Isabel</v>
       </c>
       <c r="C43" t="str">
-        <v>Isabel… petita d’alçada però gegant en somriures: el barret et veu com a…</v>
+        <v>Isabel… petita d’alçada però gegant en somriures: el barret et veu com a espurna que encén la confiança als primers intents…</v>
       </c>
       <c r="D43" t="str">
         <v>Talent emergent, persona petita i amable, sempre amb un somriure.</v>
@@ -1141,7 +1141,7 @@
         <v>Fumat</v>
       </c>
       <c r="C44" t="str">
-        <v>Fumat… xicalla, sud i castells a la sang: el barret et veu com a…</v>
+        <v>Fumat… xicalla, sud i castells a la sang: el barret et veu com a pont entre tradicions, rialles i generacions…</v>
       </c>
       <c r="D44" t="str">
         <v>Nou en l’equip de xicalla, amant dels xiquets i xiquetes i del sud del País Valencià, terra de castells.</v>
@@ -1158,7 +1158,7 @@
         <v>Amaranta</v>
       </c>
       <c r="C45" t="str">
-        <v>Amaranta… Betis, festa i faixa sense descans: el barret et proclama…</v>
+        <v>Amaranta… Betis, festa i faixa sense descans: el barret et proclama tempesta de colors verd-i-blanc en qualsevol barra de bar…</v>
       </c>
       <c r="D45" t="str">
         <v>En guany és sense dubte el fetge de festa; li agrada la festa, participar i la muixeranga; sevillana del Betis que no deixa ningú indiferent.</v>
@@ -1175,7 +1175,7 @@
         <v>Selena</v>
       </c>
       <c r="C46" t="str">
-        <v>Selena… escenari abans que assaig, somriure abans que tot: el barret et deixa a…</v>
+        <v>Selena… escenari abans que assaig, somriure abans que tot: el barret et deixa a la primera fila, allà on sempre passa alguna cosa divertida…</v>
       </c>
       <c r="D46" t="str">
         <v>Fa temps que intentem col·locar-la a prop de Sònia per muntar un grup de música; no es perd cap actuació, els assajos li costen més, però aquell somriure ho compensa.</v>
@@ -1192,7 +1192,7 @@
         <v>Nius</v>
       </c>
       <c r="C47" t="str">
-        <v>Nius… xicalla, ajuda i somriure constant: el barret et tria…</v>
+        <v>Nius… xicalla, ajuda i somriure constant: el barret et tria com aquella presència que fa que res semble tan difícil…</v>
       </c>
       <c r="D47" t="str">
         <v>Ajudanta de xicalla i amant dels xiquets i xiquetes; sempre amb somriure i ganes d’ajudar.</v>
@@ -1209,7 +1209,7 @@
         <v>Llorenç</v>
       </c>
       <c r="C48" t="str">
-        <v>Llorenç… mestre, motor i enamorat del projecte: el barret et proclama…</v>
+        <v>Llorenç… mestre, motor i enamorat del projecte: el barret et proclama cervell, cor i cronista d’esta petita bogeria col·lectiva…</v>
       </c>
       <c r="D48" t="str">
         <v>Qui està preparant la dinàmica; amant de Laura, la seua companya; va ser mestre de la muixeranga l’any passat i li agrada ajudar perquè el projecte avance.</v>
@@ -1226,7 +1226,7 @@
         <v>Mireia</v>
       </c>
       <c r="C49" t="str">
-        <v>Mireia… plaça compartida entre castells i muixerangues: el barret et posa a…</v>
+        <v>Mireia… plaça compartida entre castells i muixerangues: el barret et posa a la frontera amable on les colles es fan cosines…</v>
       </c>
       <c r="D49" t="str">
         <v>Sempre que pot ve a actuacions i assajos; castellera espectacular de l’Esquerra de l’Eixample.</v>
@@ -1243,7 +1243,7 @@
         <v>Sergi</v>
       </c>
       <c r="C50" t="str">
-        <v>Sergi… pinyes cuidades, tècnica fina i fetge provat: el barret et declara…</v>
+        <v>Sergi… pinyes cuidades, tècnica fina i fetge provat: el barret et declara responsable de que la base aguante fins i tot els dies estranys…</v>
       </c>
       <c r="D50" t="str">
         <v>Mestre l’any passat amb Llorenç; prepara les pinyes amb molt de carinyo i tècnica espectacular; l’any passat va guanyar el premi Fetge de ferro.</v>
@@ -1260,7 +1260,7 @@
         <v>Hortelano</v>
       </c>
       <c r="C51" t="str">
-        <v>Hortelano… serietat, constància i feina ben feta: el barret et veu…</v>
+        <v>Hortelano… serietat, constància i feina ben feta: el barret et veu com a exemple que els passos petits fan figures enormes…</v>
       </c>
       <c r="D51" t="str">
         <v>Fa temps que està a la colla; seriós però constant, ha aconseguit les proves que li han posat amb treball i dedicació.</v>
@@ -1277,7 +1277,7 @@
         <v>Robert</v>
       </c>
       <c r="C52" t="str">
-        <v>Robert… dels inicis i sempre present encara que siga des de fora: el barret et manté a…</v>
+        <v>Robert… dels inicis i sempre present encara que siga des de fora: el barret et manté a la sala de màquines dels records compartits…</v>
       </c>
       <c r="D52" t="str">
         <v>Ara no està a les pinyes però forma part dels inicis del projecte; s’espera tornar a veure’l prop d’una pinya.</v>
@@ -1294,7 +1294,7 @@
         <v>Cubero</v>
       </c>
       <c r="C53" t="str">
-        <v>“Cubero… cançons, paelles i missatges d’amor nocturns: el barret et proclama…”</v>
+        <v>“Cubero… cançons, paelles i missatges d’amor nocturns: el barret et proclama barda oficial de la colla, amb cassola i guitarra a punt…”</v>
       </c>
       <c r="D53" t="str">
         <v>Músic de la colla, ha fet una cançó per a vosaltres; arriba sovint borratxet a casa i envia missatges amorosos a la colla. Amant de la cuina i la paella; valencià de cor però d’Hospitalet.</v>
@@ -1311,7 +1311,7 @@
         <v>Ferran Rosell</v>
       </c>
       <c r="C54" t="str">
-        <v>“Ferran Rosell… orellut, compromès i sempre fent ponts amb Sants: el barret et veu com a…”</v>
+        <v>“Ferran Rosell… orellut, compromès i sempre fent ponts amb Sants: el barret et veu com a emissari de bona voluntat entre faixes germanes…”</v>
       </c>
       <c r="D54" t="str">
         <v>De Castelló de la Plana i del CD Castelló; talent emergent que des de l’any passat ho està donant tot i ha obert molts llaços amb els castellers de Sants.</v>
@@ -1328,7 +1328,7 @@
         <v>Paloma</v>
       </c>
       <c r="C55" t="str">
-        <v>“Paloma… baix esplèndida, somriure tranquil i ni una queixa: el barret et deixa a…”</v>
+        <v>“Paloma… baix esplèndida, somriure tranquil i ni una queixa: el barret et deixa al lloc on el pes no és només físic, sinó també emocional…”</v>
       </c>
       <c r="D55" t="str">
         <v>Gallega d’origen, mai es queixa, sempre amb somriure i disposada a fer el que calga per la muixeranga; és una baixa espectacular.</v>
@@ -1345,7 +1345,7 @@
         <v>Laura</v>
       </c>
       <c r="C56" t="str">
-        <v>“Laura Huart… cures, riures i escalfaments mítics: el barret et col·loca a…”</v>
+        <v>“Laura Huart… cures, riures i escalfaments mítics: el barret et col·loca a la línia calenta on comencen totes les històries de plaça…”</v>
       </c>
       <c r="D56" t="str">
         <v>De la comissió sanitària, vetlla per les vostres vides i és una de les persones més divertides de la colla; els seus escalfaments són inigualables.</v>
@@ -1362,7 +1362,7 @@
         <v>Mafra</v>
       </c>
       <c r="C57" t="str">
-        <v>“Mafra… diamant en brut, alçadora amb molt futur: el barret et veu com a…”</v>
+        <v>“Mafra… diamant en brut, alçadora amb molt futur: el barret et veu com a peça que encara s’està tallant però ja brilla des de lluny…”</v>
       </c>
       <c r="D57" t="str">
         <v>Talent emergent, un diamant per descobrir, amb un perfil molt bo d’alçadora i molt per aportar els pròxims mesos.</v>
@@ -1379,7 +1379,7 @@
         <v>Amparo</v>
       </c>
       <c r="C58" t="str">
-        <v>“Amparo… rialles, ‘merch’ i anys de projecte: el barret et fa…”</v>
+        <v>“Amparo… rialles, ‘merch’ i anys de projecte: el barret et fa responsable de que ningú se’n vaja a casa sense un record i una anècdota…”</v>
       </c>
       <c r="D58" t="str">
         <v>Diversió en persona, mare d’un muixeranguer i involucrada en el projecte des dels inicis; a la comissió de material ha fet que es venguen moltes més coses.</v>
@@ -1396,7 +1396,7 @@
         <v>Ferran</v>
       </c>
       <c r="C59" t="str">
-        <v>“Ferran… taladre, desfase i llegenda viva de la festa: el barret et proclama…”</v>
+        <v>“Ferran… taladre, desfase i llegenda viva de la festa: el barret et proclama protagonista d’aquelles nits que ningú acaba d’explicar senceres…”</v>
       </c>
       <c r="D59" t="str">
         <v>L’any passat va guanyar el premi al personatge de l’any (molt disputat amb Carles); amb el seu desfase de festa i el taladre guanyat en un concurs sempre deixa tothom bocabadat.</v>
@@ -1413,7 +1413,7 @@
         <v>Shannon</v>
       </c>
       <c r="C60" t="str">
-        <v>Shannon… mig cor a Califòrnia i mig a la plaça: el barret et veu com a…</v>
+        <v>Shannon… mig cor a Califòrnia i mig a la plaça: el barret et veu com a pont oceànic que porta accent nou i abraçades velles…</v>
       </c>
       <c r="D60" t="str">
         <v>De Califòrnia, una de les membres més internacionals; fa temps que és amb vosaltres i sempre que pot ve a donar un cop de mà.</v>
@@ -1430,7 +1430,7 @@
         <v>Lloret</v>
       </c>
       <c r="C61" t="str">
-        <v>Lloret… saforí, graciós i una mica desaparegut de tant en tant: el barret et declara…</v>
+        <v>Lloret… saforí, graciós i una mica desaparegut de tant en tant: el barret et declara cometa que apareix per il·luminar un parell de nits l’any…</v>
       </c>
       <c r="D61" t="str">
         <v>El tio més salat de la colla, pare de família, molt divertit, de la Safor, cor del País Valencià; de vegades us deixa tirats a última hora, però la seua presència sempre paga la pena.</v>
@@ -1447,7 +1447,7 @@
         <v>Xavi</v>
       </c>
       <c r="C62" t="str">
-        <v>Xavi… faixes, família i mirada crítica que fa créixer: el barret et deixa a…</v>
+        <v>Xavi… faixes, família i mirada crítica que fa créixer: el barret et deixa a la taula on es prenen les decisions difícils amb molt de carinyo…</v>
       </c>
       <c r="D62" t="str">
         <v>Pare de família i segon president de la Muixeranga de Barcelona; sempre compromés amb el projecte i amb un punt de crítica constructiva molt valuós.</v>
@@ -1464,7 +1464,7 @@
         <v>Alfred</v>
       </c>
       <c r="C63" t="str">
-        <v>Alfred… joventut castellonenca i ofici de La Plana: el barret et veu com a…</v>
+        <v>Alfred… joventut castellonenca i ofici de La Plana: el barret et veu com a record vivent que el poble sempre es porta a sobre…</v>
       </c>
       <c r="D63" t="str">
         <v>Fins fa poc el més jove de la colla; castellonenc que abans feia Muixeranga La Plana, amb trajectòria i arrels muixerangueres.</v>
@@ -1481,7 +1481,7 @@
         <v>Gerard</v>
       </c>
       <c r="C64" t="str">
-        <v>Gerard… Sueca al cor, hiperactivitat amable i sempre un pla nou: el barret et posa a…</v>
+        <v>Gerard… Sueca al cor, hiperactivitat amable i sempre un pla nou: el barret et posa en temporada permanent de propostes i improvisacions…</v>
       </c>
       <c r="D64" t="str">
         <v>Saforenc de Sueca, on el valencià no és cap dubte; improvisador i hiperactiu amable, ha portat família i alumnes a la muixeranga.</v>
@@ -1498,7 +1498,7 @@
         <v>Wendy</v>
       </c>
       <c r="C65" t="str">
-        <v>Wendy… aire fresc, pas ferm i futur per escriure: el barret et veu com a…</v>
+        <v>Wendy… aire fresc, pas ferm i futur per escriure: el barret et veu com a pàgina en blanc plena de possibilitats muixerangueres…</v>
       </c>
       <c r="D65" t="str">
         <v>Talent emergent que aporta aire fresc a la colla; teniu molt bones expectatives posades en ella.</v>
@@ -1515,7 +1515,7 @@
         <v>Núria</v>
       </c>
       <c r="C66" t="str">
-        <v>Núria… dels inicis, ara a la reserva però mai lluny del cor de la colla: el barret et deixa a…</v>
+        <v>Núria… dels inicis, ara a la reserva però mai lluny del cor de la colla: el barret et deixa al lloc on s’arxiven les històries més tendres…</v>
       </c>
       <c r="D66" t="str">
         <v>Des de l’inici del projecte amb vosaltres; ara mare de dos xiquets, està a la reserva però sempre esperant tornar.</v>
@@ -1532,7 +1532,7 @@
         <v>Blai</v>
       </c>
       <c r="C67" t="str">
-        <v>Blai… quatre anyets i mil idees al cap: el barret et proclama…</v>
+        <v>Blai… quatre anyets i mil idees al cap: el barret et proclama narrador en miniatura de coses que els adults ni tan sols veiem…</v>
       </c>
       <c r="D67" t="str">
         <v>Fill de Núria, xicalla i futur de la colla; sempre diu coses molt curioses tot i tindre quatre anys, és un amor.</v>
@@ -1549,7 +1549,7 @@
         <v>Aloma</v>
       </c>
       <c r="C68" t="str">
-        <v>Aloma… curiositat als ulls i enamorament en marxa: el barret et veu com a…</v>
+        <v>Aloma… curiositat als ulls i enamorament en marxa: el barret et veu com a llavor que ja ha trobat la seua terra…</v>
       </c>
       <c r="D68" t="str">
         <v>Xiqueta que comença a enamorar-se de la muixeranga; tota la colla té molta il·lusió que li agrade cada vegada més i s’integre.</v>
@@ -1566,7 +1566,7 @@
         <v>Pol</v>
       </c>
       <c r="C69" t="str">
-        <v>Pol… enano de naixement muixeranguer, broma constant i carisma infantil: el barret et posa a…</v>
+        <v>Pol… enano de naixement muixeranguer, broma constant i carisma infantil: el barret et posa al centre de totes les rialles petites…</v>
       </c>
       <c r="D69" t="str">
         <v>Un dels grans personatges de la colla; el més divertit dels xiquets, criat entre muixerangues des que és molt menut, sempre gastant bromes i molt estimat.</v>
@@ -1583,7 +1583,7 @@
         <v>Joan</v>
       </c>
       <c r="C70" t="str">
-        <v>Joan… de xicalla fundadora a pinya i suport: el barret et declara…</v>
+        <v>Joan… de xicalla fundadora a pinya i suport: el barret et declara pont entre el que éreu i el que sou ara…</v>
       </c>
       <c r="D70" t="str">
         <v>Germà de Pol; ja no és xicalla, ha passat a fer pinya i ajudar a la xicalla. Va ser a la colla des de la seua creació fins avui.</v>
@@ -1600,7 +1600,7 @@
         <v>Lina</v>
       </c>
       <c r="C71" t="str">
-        <v>Lina… colors a la cara, pilars ferms i anys de dedicació: el barret et tria…</v>
+        <v>Lina… colors a la cara, pilars ferms i anys de dedicació: el barret et tria com a artista de fons que fa que tot siga més bonic…</v>
       </c>
       <c r="D71" t="str">
         <v>D’Equador, fa molts anys que pertany a la colla; sempre disposada a fer un piló i a pintar les cares de la xicalla.</v>
@@ -1617,7 +1617,7 @@
         <v>Martí</v>
       </c>
       <c r="C72" t="str">
-        <v>Martí… energia desbordada i mans de músic en potència: el barret et col·loca a…</v>
+        <v>Martí… energia desbordada i mans de músic en potència: el barret et col·loca a la banda sonora sorollosa però imprescindible de la colla…</v>
       </c>
       <c r="D72" t="str">
         <v>Fill de Lina i Lloret; és un terremoto, potser no és el xiquet que més li agrada la muixeranga, però si li dones un tabal serà el vostre músic. Molt estimat per tothom.</v>
@@ -1626,9 +1626,14 @@
         <v>Comboiet</v>
       </c>
     </row>
+    <row r="73">
+      <c r="C73" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E72"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E73"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>